<commit_message>
altre prove di pesi
</commit_message>
<xml_diff>
--- a/submission/RIEPILOGO PESI.xlsx
+++ b/submission/RIEPILOGO PESI.xlsx
@@ -388,7 +388,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,6 +432,9 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>503</v>
+      </c>
       <c r="C5">
         <v>482</v>
       </c>

</xml_diff>